<commit_message>
plot updates for FALO and DRKAT
Just need to add post-data
</commit_message>
<xml_diff>
--- a/data/prge_brief_self.xlsx
+++ b/data/prge_brief_self.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon/BrICC Clinic/BrICC Terms/Spring 2020/pilot_data_2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD4FFCD-2DEA-1841-9F22-329184C63929}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB53688F-DA88-0545-A103-48C1E8126A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35100" yWindow="6480" windowWidth="27640" windowHeight="15760" xr2:uid="{11FF7B4C-1621-664D-9969-2BAB396DB739}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>